<commit_message>
fixed form3 diem danh khi chua mo
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/Debug/Data/Data.xlsx
+++ b/WindowsFormsApp2/bin/Debug/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PM Diem Danh\WindowsFormsApp2\bin\Debug\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EF4A375F-5302-45DF-A321-555C2EE5B1F5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{581FC7C3-0515-428D-8EEA-F02AD864F9AE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9285096D-E9BE-4E31-B3A9-605255BE9D86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>STT</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>C2</t>
+  </si>
+  <si>
+    <t>Thoi gian</t>
   </si>
 </sst>
 </file>
@@ -558,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BD5EE9-9FDF-410A-AF22-839293E087A2}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,10 +575,11 @@
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="23.28515625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,8 +598,11 @@
       <c r="F1" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -615,7 +622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -635,7 +642,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -655,7 +662,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -675,7 +682,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -695,7 +702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -715,7 +722,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -735,7 +742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -755,7 +762,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -775,7 +782,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -795,7 +802,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -815,7 +822,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -835,11 +842,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>3113410024</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -855,14 +862,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>

</xml_diff>